<commit_message>
Added Gerbers for mini cape rev. B2, updated BOM, and created an EAGLE CAM job for the mini cape.
</commit_message>
<xml_diff>
--- a/pocketbela-cape/belamini_cape_rev_B2/belamini_cape_B2_bom.xlsx
+++ b/pocketbela-cape/belamini_cape_rev_B2/belamini_cape_B2_bom.xlsx
@@ -281,10 +281,10 @@
     <t>36-pin header</t>
   </si>
   <si>
-    <t>2x18 2.54mm stacking headers (long male pins on bottom, female sockets on top).</t>
-  </si>
-  <si>
-    <t>Important: use 9mm pin length rather than 12mm used on previous Bela builds</t>
+    <t>2x18 2.54mm stacking headers (10mm male pins on bottom, female sockets on top).</t>
+  </si>
+  <si>
+    <t>Important: use 10mm pin length rather than 12.5mm used on previous Bela builds</t>
   </si>
   <si>
     <t>R1, R2</t>
@@ -335,7 +335,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>BOM rev. B1</t>
+    <t>BOM rev. B2</t>
   </si>
 </sst>
 </file>

</xml_diff>